<commit_message>
Made updates to align with the rewrite of reach-silabs
</commit_message>
<xml_diff>
--- a/nRF52840 Dongle Demo.xlsx
+++ b/nRF52840 Dongle Demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseph.peplinski\Reach\reach-nrfc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48868DA-BED4-410E-AF28-4A22A92E5AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E668B4-225D-4080-90AF-A301AA7DC237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10090" yWindow="-21710" windowWidth="38620" windowHeight="21220" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device Information" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="73">
   <si>
     <t>Device Name</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>White</t>
+  </si>
+  <si>
+    <t>Click for Wisdom</t>
   </si>
 </sst>
 </file>
@@ -7760,8 +7763,8 @@
   </sheetPr>
   <dimension ref="A1:B995"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7802,7 +7805,9 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+      <c r="A5" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="B5" s="4"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -13860,7 +13865,7 @@
   </sheetPr>
   <dimension ref="A1:B999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated advertisements to work better with iOS and without requiring SDK changes
</commit_message>
<xml_diff>
--- a/nRF52840 Dongle Demo.xlsx
+++ b/nRF52840 Dongle Demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseph.peplinski\Reach\reach-nrfc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E668B4-225D-4080-90AF-A301AA7DC237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FA9994-2937-49A8-A0FF-EE98D3AB5689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2292" yWindow="1188" windowWidth="19176" windowHeight="10296" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device Information" sheetId="1" r:id="rId1"/>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>string</t>
-  </si>
-  <si>
-    <t>Up to 26 characters</t>
   </si>
   <si>
     <t>Read/Write</t>
@@ -244,6 +241,9 @@
   </si>
   <si>
     <t>Click for Wisdom</t>
+  </si>
+  <si>
+    <t>Up to 29 characters</t>
   </si>
 </sst>
 </file>
@@ -618,9 +618,9 @@
   </sheetPr>
   <dimension ref="A1:Z141"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -674,18 +674,18 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="5"/>
       <c r="K2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
@@ -705,17 +705,17 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4">
@@ -723,26 +723,26 @@
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H4" s="4">
         <v>-43200</v>
@@ -754,15 +754,15 @@
         <v>43200</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -771,166 +771,166 @@
         <v>6</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H12" s="4">
         <v>0.01</v>
@@ -942,7 +942,7 @@
         <v>60</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
@@ -2713,44 +2713,44 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="4">
         <v>458240</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="4">
         <v>512</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="4">
         <v>17900</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -7763,7 +7763,7 @@
   </sheetPr>
   <dimension ref="A1:B995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -7782,31 +7782,31 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="4" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B3" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="B4" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="4"/>
     </row>
@@ -10821,49 +10821,49 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="4"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="4"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="4"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="4"/>
     </row>
@@ -13881,19 +13881,19 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="4"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>65</v>
-      </c>
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="4"/>
     </row>

</xml_diff>